<commit_message>
a bunch of changes to handle validation of empty values properly
</commit_message>
<xml_diff>
--- a/bmh_sample_tracker/static/sample_sheet.xlsx
+++ b/bmh_sample_tracker/static/sample_sheet.xlsx
@@ -42,16 +42,16 @@
     <t xml:space="preserve">requested_services</t>
   </si>
   <si>
+    <t xml:space="preserve">genus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species</t>
+  </si>
+  <si>
     <t xml:space="preserve">strain</t>
   </si>
   <si>
     <t xml:space="preserve">isolate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">species</t>
   </si>
   <si>
     <t xml:space="preserve">subspecies_subtype_lineage</t>
@@ -245,8 +245,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -353,7 +353,7 @@
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -364,10 +364,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="41.85"/>
@@ -398,10 +398,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -455,16 +455,16 @@
         <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>25</v>
@@ -666,7 +666,7 @@
     <row r="37" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="I37" s="5"/>
       <c r="N37" s="4"/>
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
@@ -722,8 +722,8 @@
       <c r="AMJ47" s="0"/>
     </row>
   </sheetData>
-  <dataValidations count="19">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="If submitting tubes, enter the tube name.&#10;If submitting plates, specify the well (ex: A1, H12, etc)." promptTitle="well:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:C1" type="none">
+  <dataValidations count="17">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="If submitting tubes, enter the tube name.&#10;If submitting plates, specify the well (ex: A1, H12, etc)." promptTitle="well:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:C1 G1:H1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -743,19 +743,11 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the strain name if known. " promptTitle="Strain" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the isolate name. This is often the same as the sample name, but we can distinguish isolates by culture date if needed. " promptTitle="Isolate:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the genus if known." promptTitle="Genus:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I1" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the species if known" promptTitle="Species:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J1" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the strain name if known. " promptTitle="Strain" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I1" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the isolate name. This is often the same as the sample name, but we can distinguish isolates by culture date if needed. " promptTitle="Isolate:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
update sample sheet template
</commit_message>
<xml_diff>
--- a/bmh_sample_tracker/static/sample_sheet.xlsx
+++ b/bmh_sample_tracker/static/sample_sheet.xlsx
@@ -9,9 +9,15 @@
   </bookViews>
   <sheets>
     <sheet name="SSS-Template" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="sample_type_List" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="requested_services_list" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="submitting_lab_List" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="sample_type_List" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="requested_services_list" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="ProjectID_List" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">submitting_lab_List!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">ProjectID_List!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
   <si>
     <t xml:space="preserve">sample_name</t>
   </si>
@@ -42,18 +48,18 @@
     <t xml:space="preserve">requested_services</t>
   </si>
   <si>
+    <t xml:space="preserve">strain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isolate</t>
+  </si>
+  <si>
     <t xml:space="preserve">genus</t>
   </si>
   <si>
     <t xml:space="preserve">species</t>
   </si>
   <si>
-    <t xml:space="preserve">strain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isolate</t>
-  </si>
-  <si>
     <t xml:space="preserve">subspecies_subtype_lineage</t>
   </si>
   <si>
@@ -93,6 +99,9 @@
     <t xml:space="preserve">Illumina WGS</t>
   </si>
   <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Escherichia</t>
   </si>
   <si>
@@ -105,10 +114,49 @@
     <t xml:space="preserve">test data, do not use</t>
   </si>
   <si>
-    <t xml:space="preserve">describe culture conditions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phenol chloroform</t>
+    <t xml:space="preserve">Enter culture details (media, time, temp, etc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if applicable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submitting_lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Botulism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parasitology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapid-Diagnostics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vibrio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genomics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Added Dec 14/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other - specify in comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Amended Dec 14/2020</t>
   </si>
   <si>
     <t xml:space="preserve">DNA</t>
@@ -117,6 +165,9 @@
     <t xml:space="preserve">RNA</t>
   </si>
   <si>
+    <t xml:space="preserve">* Added Dec 14/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amplicon - details in comments</t>
   </si>
   <si>
@@ -136,16 +187,137 @@
   </si>
   <si>
     <t xml:space="preserve">Other (specify in comments)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProjectIDs in Portal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRS2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRS2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human_Study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brooks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOD-Mice_2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unidentified_Data_Sets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KT_Proficiency_2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listeria2016WGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listeria2018WGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listeria2019WGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listeria-Food_2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LRS_Coleslaw1981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LRS_Staph_CBS_2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIARDIA2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIARDIA2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapid_Diagnostics_2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChickenNugget2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FoodNet2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRDI-AMR_DNAKitEval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRDI-AMR_metagenomics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRDI-AMR_Recip2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRDI-AMR_RetailMeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oyster2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sal_Chia_2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sal_Profiterole2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shigella2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019_Bacillus_Shwed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shwed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRDI-AMR_Aeromonas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRDI-AMR_VIBRIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAV-SPIKED_FOODS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norovirus_AmpliconWGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100D-SNP_2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LactoseFermentation2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stx-subtype_2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTEC_FLOUR_2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTEC-RMCheese_2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other - TBD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="166" formatCode="mmm/yy"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="167" formatCode="mmm/yy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -240,13 +412,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -265,7 +437,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -282,6 +462,23 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF3D3D3D"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -353,7 +550,7 @@
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -364,10 +561,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="41.85"/>
@@ -398,10 +595,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -455,37 +652,37 @@
         <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" s="3" t="n">
         <v>5600000</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" s="4" t="n">
         <v>43831</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="4" t="n">
-        <v>43832</v>
+        <v>28</v>
+      </c>
+      <c r="P2" s="5" t="n">
+        <v>43831</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R2" s="3" t="n">
         <v>1</v>
@@ -664,9 +861,9 @@
       <c r="AMJ36" s="0"/>
     </row>
     <row r="37" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="I37" s="5"/>
+      <c r="A37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="G37" s="6"/>
       <c r="N37" s="4"/>
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
@@ -722,8 +919,8 @@
       <c r="AMJ47" s="0"/>
     </row>
   </sheetData>
-  <dataValidations count="17">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="If submitting tubes, enter the tube name.&#10;If submitting plates, specify the well (ex: A1, H12, etc)." promptTitle="well:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:C1 G1:H1" type="none">
+  <dataValidations count="19">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="If submitting tubes, enter the tube name.&#10;If submitting plates, specify the well (ex: A1, H12, etc)." promptTitle="well:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:C1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -743,11 +940,19 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the strain name if known. " promptTitle="Strain" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I1" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the isolate name. This is often the same as the sample name, but we can distinguish isolates by culture date if needed. " promptTitle="Isolate:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J1" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the strain name if known. " promptTitle="Strain" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the isolate name. This is often the same as the sample name, but we can distinguish isolates by culture date if needed. " promptTitle="Isolate:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the genus if known." promptTitle="Genus:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I1" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter the species if known" promptTitle="Species:" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -807,57 +1012,98 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="A1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -874,6 +1120,80 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -894,24 +1214,351 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>